<commit_message>
Create a second sheet in the Excel workbook that stack ranks accounts for the search keyword
</commit_message>
<xml_diff>
--- a/email-builder-output.xlsx
+++ b/email-builder-output.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="DataMiner-spring-and-java.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" r:id="rId6" sheetId="2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10724" uniqueCount="5717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10836" uniqueCount="5761">
   <si>
     <t>Full Name Displayed</t>
   </si>
@@ -17170,6 +17171,138 @@
   </si>
   <si>
     <t>Stephen_Hanek@homedepot.com</t>
+  </si>
+  <si>
+    <t>Total Found</t>
+  </si>
+  <si>
+    <t>ups.com</t>
+  </si>
+  <si>
+    <t>danaher.com</t>
+  </si>
+  <si>
+    <t>chicos.com</t>
+  </si>
+  <si>
+    <t>southernco.com</t>
+  </si>
+  <si>
+    <t>markelcorp.com</t>
+  </si>
+  <si>
+    <t>genworth.com</t>
+  </si>
+  <si>
+    <t>inovalon.com</t>
+  </si>
+  <si>
+    <t>sbgnet.com</t>
+  </si>
+  <si>
+    <t>hanloninvest.com</t>
+  </si>
+  <si>
+    <t>merck.com</t>
+  </si>
+  <si>
+    <t>nielsen.com</t>
+  </si>
+  <si>
+    <t>altisource.com</t>
+  </si>
+  <si>
+    <t>microstrategy.com</t>
+  </si>
+  <si>
+    <t>freedommortgage.com</t>
+  </si>
+  <si>
+    <t>masonite.com</t>
+  </si>
+  <si>
+    <t>autonation.com</t>
+  </si>
+  <si>
+    <t>astrazeneca.com</t>
+  </si>
+  <si>
+    <t>sykes.com</t>
+  </si>
+  <si>
+    <t>slhn.org</t>
+  </si>
+  <si>
+    <t>subaru.com</t>
+  </si>
+  <si>
+    <t>footballfanatics.com</t>
+  </si>
+  <si>
+    <t>carmax.com</t>
+  </si>
+  <si>
+    <t>bbandt.com</t>
+  </si>
+  <si>
+    <t>aflac.com</t>
+  </si>
+  <si>
+    <t>baycare.org</t>
+  </si>
+  <si>
+    <t>troweprice.com</t>
+  </si>
+  <si>
+    <t>vertexinc.com</t>
+  </si>
+  <si>
+    <t>iassoftware.com</t>
+  </si>
+  <si>
+    <t>tsys.com</t>
+  </si>
+  <si>
+    <t>carnival.com</t>
+  </si>
+  <si>
+    <t>darden.com</t>
+  </si>
+  <si>
+    <t>ahss.org</t>
+  </si>
+  <si>
+    <t>syniverse.com</t>
+  </si>
+  <si>
+    <t>nascar.com</t>
+  </si>
+  <si>
+    <t>wellcare.com</t>
+  </si>
+  <si>
+    <t>mohawkind.com</t>
+  </si>
+  <si>
+    <t>transcore.com</t>
+  </si>
+  <si>
+    <t>carecorenational.com</t>
+  </si>
+  <si>
+    <t>usa.dupont.com</t>
+  </si>
+  <si>
+    <t>ultimatesoftware.com</t>
+  </si>
+  <si>
+    <t>fticonsulting.com</t>
+  </si>
+  <si>
+    <t>benefitfocus.com</t>
+  </si>
+  <si>
+    <t>praintl.com</t>
   </si>
 </sst>
 </file>
@@ -47927,4 +48060,909 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="21.8984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.63671875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>3608</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5717</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3692</v>
+      </c>
+      <c r="B2" t="n">
+        <v>135.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3730</v>
+      </c>
+      <c r="B3" t="n">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3631</v>
+      </c>
+      <c r="B4" t="n">
+        <v>44.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3664</v>
+      </c>
+      <c r="B5" t="n">
+        <v>37.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B6" t="n">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>3654</v>
+      </c>
+      <c r="B7" t="n">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>3778</v>
+      </c>
+      <c r="B8" t="n">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>3809</v>
+      </c>
+      <c r="B9" t="n">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>3675</v>
+      </c>
+      <c r="B10" t="n">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>3711</v>
+      </c>
+      <c r="B11" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>4013</v>
+      </c>
+      <c r="B12" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>3715</v>
+      </c>
+      <c r="B13" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B14" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>3942</v>
+      </c>
+      <c r="B15" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>3798</v>
+      </c>
+      <c r="B16" t="n">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>3986</v>
+      </c>
+      <c r="B17" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>3650</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>3772</v>
+      </c>
+      <c r="B19" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>4675</v>
+      </c>
+      <c r="B20" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>3979</v>
+      </c>
+      <c r="B21" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>3965</v>
+      </c>
+      <c r="B22" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>4140</v>
+      </c>
+      <c r="B23" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>3699</v>
+      </c>
+      <c r="B24" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>3793</v>
+      </c>
+      <c r="B25" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>4071</v>
+      </c>
+      <c r="B26" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>3616</v>
+      </c>
+      <c r="B27" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>3734</v>
+      </c>
+      <c r="B28" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>3612</v>
+      </c>
+      <c r="B29" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>3702</v>
+      </c>
+      <c r="B30" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>3620</v>
+      </c>
+      <c r="B31" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>3627</v>
+      </c>
+      <c r="B32" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>4075</v>
+      </c>
+      <c r="B33" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B34" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>3846</v>
+      </c>
+      <c r="B35" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B36" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>3719</v>
+      </c>
+      <c r="B37" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>4424</v>
+      </c>
+      <c r="B38" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>3923</v>
+      </c>
+      <c r="B39" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>4195</v>
+      </c>
+      <c r="B40" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>3916</v>
+      </c>
+      <c r="B41" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>3969</v>
+      </c>
+      <c r="B42" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>4427</v>
+      </c>
+      <c r="B43" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>4188</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>4713</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>3643</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>4433</v>
+      </c>
+      <c r="B48" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>4394</v>
+      </c>
+      <c r="B49" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>4225</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>4390</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>5061</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>4103</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>4338</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>4402</v>
+      </c>
+      <c r="B55" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>3910</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>4569</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>4064</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>5022</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>4541</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>5076</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>5125</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>5103</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>5030</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>5240</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>4454</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>4777</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>3824</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>5718</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>5719</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>5720</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>5721</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>5722</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>5723</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>5724</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>5725</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>5726</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>5727</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>5728</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>5729</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>5730</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>5731</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>5732</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>5733</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>5734</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>5735</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>5736</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>5737</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>5738</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>5739</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>5740</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>5741</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>5742</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>5743</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>5744</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>5745</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>5746</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>5747</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>5748</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>5749</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>5750</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>5751</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>5752</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>5753</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>5754</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>5755</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>5756</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>5757</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>5758</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>5759</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>5760</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for account Audi of America and Volkswagen Group of America
</commit_message>
<xml_diff>
--- a/email-builder-output.xlsx
+++ b/email-builder-output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10836" uniqueCount="5761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10838" uniqueCount="5763">
   <si>
     <t>Full Name Displayed</t>
   </si>
@@ -17191,6 +17191,9 @@
     <t>markelcorp.com</t>
   </si>
   <si>
+    <t>vw.com</t>
+  </si>
+  <si>
     <t>genworth.com</t>
   </si>
   <si>
@@ -17246,6 +17249,9 @@
   </si>
   <si>
     <t>aflac.com</t>
+  </si>
+  <si>
+    <t>audiusa.com</t>
   </si>
   <si>
     <t>baycare.org</t>
@@ -48962,6 +48968,22 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>5761</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>5762</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Create new sheet in output Excel workbook to eventually hold output data formatted to be delivered to marketing for upload to SFDC
</commit_message>
<xml_diff>
--- a/email-builder-output.xlsx
+++ b/email-builder-output.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Named Accounts" sheetId="2" r:id="rId2"/>
     <sheet name="Email Types" sheetId="3" r:id="rId3"/>
     <sheet name="Summary" r:id="rId8" sheetId="4"/>
+    <sheet name="Marketo" r:id="rId9" sheetId="5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Named Accounts'!$A$6:$F$138</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11244" uniqueCount="6020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11264" uniqueCount="6040">
   <si>
     <t>Full Name Displayed</t>
   </si>
@@ -18085,6 +18086,66 @@
   </si>
   <si>
     <t>Total Found</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Original Lead Source Description</t>
+  </si>
+  <si>
+    <t>Original Lead Source</t>
+  </si>
+  <si>
+    <t>Most Recent Lead Source</t>
+  </si>
+  <si>
+    <t>Most Recent Lead Source Description</t>
+  </si>
+  <si>
+    <t>Lead Action</t>
+  </si>
+  <si>
+    <t>Agile</t>
+  </si>
+  <si>
+    <t>Product: Data</t>
+  </si>
+  <si>
+    <t>PaaS</t>
+  </si>
+  <si>
+    <t>Labs</t>
+  </si>
+  <si>
+    <t>PWS</t>
   </si>
 </sst>
 </file>
@@ -52331,4 +52392,101 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="9.765625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.48828125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.921875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.359375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="7.6953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.04296875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="5.15625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.51953125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="7.4375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="27.3515625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="17.6015625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="21.56640625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="31.3125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="10.4765625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="4.953125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="12.1484375" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="4.8125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="4.57421875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="4.67578125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>6020</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6021</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6022</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6023</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6024</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6025</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6026</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6027</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6028</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6029</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6030</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6031</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6032</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6033</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6034</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6035</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6036</v>
+      </c>
+      <c r="R1" t="s">
+        <v>6037</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6038</v>
+      </c>
+      <c r="T1" t="s">
+        <v>6039</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>